<commit_message>
Clean-up en hashing PW
</commit_message>
<xml_diff>
--- a/SQl export/inhoud overzicht tabellen.xlsx
+++ b/SQl export/inhoud overzicht tabellen.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="120" windowWidth="21075" windowHeight="10035"/>
@@ -11,12 +11,12 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>leerlingnummer</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Jansen</t>
   </si>
   <si>
-    <t>Testkees</t>
-  </si>
-  <si>
     <t>Moderator</t>
   </si>
   <si>
@@ -139,13 +136,28 @@
   </si>
   <si>
     <t>(leeg)</t>
+  </si>
+  <si>
+    <t>TestKees</t>
+  </si>
+  <si>
+    <t>row6</t>
+  </si>
+  <si>
+    <t>121212</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Aartsma</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,7 +204,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -266,7 +278,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -301,7 +312,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -477,14 +487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
@@ -493,17 +503,17 @@
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -520,9 +530,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -540,135 +550,155 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>23</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" t="s">
-        <v>25</v>
       </c>
       <c r="F8">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="B14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="C14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F14" t="s">
         <v>29</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G14" t="s">
         <v>30</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H14" t="s">
         <v>31</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I14" t="s">
         <v>32</v>
       </c>
-      <c r="I13" t="s">
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -677,24 +707,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>